<commit_message>
Alterar caso de teste sussecceful login
</commit_message>
<xml_diff>
--- a/Cenários Site Adopet.xlsx
+++ b/Cenários Site Adopet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b169d1433ded32a3/Área de Trabalho/Carreia Teste/Curso-Alura-QA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="125" documentId="8_{D27B2583-B550-4A04-BC8E-FF88AA5B0BC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F2F8B730-C95D-4584-B903-4C045926D2CC}"/>
+  <xr:revisionPtr revIDLastSave="126" documentId="8_{D27B2583-B550-4A04-BC8E-FF88AA5B0BC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AB392883-C5BB-4B30-9B93-C3926631F180}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{ADC66806-1CC5-4315-B284-C5D538311E4C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{ADC66806-1CC5-4315-B284-C5D538311E4C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sucesso" sheetId="2" r:id="rId1"/>
@@ -177,95 +177,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Dado </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">que o usuário clique em "Já tenho conta"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Quando</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> inserir um usuário e senha válidos 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>E</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> clicar em "Entrar"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Então</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ele deve ser redirecionado para a página de adoção de pets</t>
-    </r>
-  </si>
-  <si>
     <t>002-Register</t>
   </si>
   <si>
@@ -781,6 +692,106 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> deve ser apresentado a menssagem de "caracter inválido"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Dado </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>que o usuário esteja na tela home e clique em "Já tenho conta"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Quando </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">inserir um usuário e senha válidos na tela de login </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+E </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>clicar em "Entrar"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Então </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">ele deve ser redirecionado para a página de adoção “pets”  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
     </r>
   </si>
 </sst>
@@ -1052,10 +1063,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1063,11 +1071,14 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1385,8 +1396,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B8BA81D-B32B-4256-8522-2F6017635661}">
   <dimension ref="A1:D295"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1419,7 +1430,7 @@
         <v>11</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D2" s="13" t="s">
         <v>4</v>
@@ -1427,7 +1438,7 @@
     </row>
     <row r="3" spans="1:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>10</v>
@@ -1440,26 +1451,26 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="30" t="s">
-        <v>19</v>
+      <c r="A4" s="25" t="s">
+        <v>18</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="27"/>
+      <c r="A5" s="26"/>
       <c r="B5" s="13" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>4</v>
@@ -3218,7 +3229,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50F99F60-8CCF-4B88-8E7E-585E00085B1E}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4:A6"/>
     </sheetView>
   </sheetViews>
@@ -3245,40 +3256,40 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="26" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="17" t="s">
         <v>14</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" s="19" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3" s="28"/>
+      <c r="A3" s="27"/>
       <c r="B3" s="17" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" s="12" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="25" t="s">
-        <v>18</v>
+      <c r="A4" s="28" t="s">
+        <v>17</v>
       </c>
       <c r="B4" s="21" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" s="12" t="s">
         <v>4</v>
@@ -3290,19 +3301,19 @@
         <v>7</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="26"/>
+      <c r="A6" s="30"/>
       <c r="B6" s="22" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D6" s="24" t="s">
         <v>9</v>

</xml_diff>